<commit_message>
Now model is working, but no good results
</commit_message>
<xml_diff>
--- a/InputDoc/EvapStruc.xlsx
+++ b/InputDoc/EvapStruc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -32,25 +32,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
-    <t>the followings are node information</t>
-  </si>
-  <si>
-    <t>the following are branch information</t>
-  </si>
-  <si>
-    <t>the following are tube information</t>
-  </si>
-  <si>
     <t>node number (headers)</t>
   </si>
   <si>
-    <t>branch number</t>
-  </si>
-  <si>
     <t>row number</t>
-  </si>
-  <si>
-    <t>tube number</t>
   </si>
   <si>
     <t>segment number of per tube</t>
@@ -129,6 +114,21 @@
   </si>
   <si>
     <t>even</t>
+  </si>
+  <si>
+    <t>please see sheet "node" for more information about the headers</t>
+  </si>
+  <si>
+    <t>branch number (circuit)</t>
+  </si>
+  <si>
+    <t>tube number (total)</t>
+  </si>
+  <si>
+    <t>please see sheet "branch" for more information about the circuits</t>
+  </si>
+  <si>
+    <t>please see sheet "tube"for more information about the tube</t>
   </si>
 </sst>
 </file>
@@ -505,17 +505,17 @@
   <dimension ref="A1:P110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -531,7 +531,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -539,7 +539,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>0.36230000000000001</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -571,12 +571,12 @@
         <v>0.94389999999999996</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -645,7 +645,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -950,30 +950,30 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" t="s">
+      <c r="G20" t="s">
         <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
@@ -2704,13 +2704,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2794,16 +2794,16 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3127,7 +3127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -3139,25 +3139,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>